<commit_message>
Add Auto Convert Snackcase
</commit_message>
<xml_diff>
--- a/EpPlus.PackageReader/TestModel/Book1.xlsx
+++ b/EpPlus.PackageReader/TestModel/Book1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diep\source\repos\EpPlus.PackageReader\EpPlus.PackageReader\TestModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E6479B-01F5-4D96-A67D-8A6215A65193}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537283D4-7119-4E23-A717-0C48FC99E436}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F5774E79-157F-4B74-BF06-4C472DF74A1C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{F5774E79-157F-4B74-BF06-4C472DF74A1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
   <si>
     <t>A2</t>
   </si>
@@ -101,12 +102,48 @@
 With special headers
 [pp] *';\":/?.&gt;,&lt;\\=+-_~`!@#$%^&amp;*()|</t>
   </si>
+  <si>
+    <t>Header 1</t>
+  </si>
+  <si>
+    <t>Header 5</t>
+  </si>
+  <si>
+    <t>Header 6</t>
+  </si>
+  <si>
+    <t>Header 7</t>
+  </si>
+  <si>
+    <t>Header 8</t>
+  </si>
+  <si>
+    <t>Header 9</t>
+  </si>
+  <si>
+    <t>Group 1</t>
+  </si>
+  <si>
+    <t>Group 2</t>
+  </si>
+  <si>
+    <t>TEST IMPORT TEMPLATE 2</t>
+  </si>
+  <si>
+    <t>Header 3*</t>
+  </si>
+  <si>
+    <t>header 1</t>
+  </si>
+  <si>
+    <t>can auto convert to SNAKE cAsE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,8 +161,49 @@
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,6 +213,22 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -277,10 +371,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -288,6 +384,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -324,8 +421,25 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -640,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2528AEA8-FEB8-415E-B7FF-CF6DCB8E9477}">
   <dimension ref="A3:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,7 +767,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -667,7 +781,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="12"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
@@ -679,7 +793,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -691,7 +805,7 @@
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="12"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="3" t="s">
         <v>2</v>
       </c>
@@ -703,10 +817,10 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="16"/>
+      <c r="C7" s="17"/>
       <c r="D7" s="4">
         <v>43466</v>
       </c>
@@ -715,54 +829,54 @@
       </c>
     </row>
     <row r="9" spans="1:18" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12" t="s">
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="5" t="s">
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="8"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12" t="s">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12" t="s">
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12" t="s">
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="13" t="s">
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="14" t="s">
         <v>4</v>
       </c>
       <c r="M10" s="2" t="s">
@@ -771,13 +885,13 @@
       <c r="N10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O10" s="8"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="10"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="11"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
@@ -805,8 +919,8 @@
       <c r="J11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
       <c r="M11" s="2" t="s">
         <v>14</v>
       </c>
@@ -2056,4 +2170,2077 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB553E4-8B26-457B-9AE4-2B0856153E13}">
+  <dimension ref="A1:BL11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B1" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+    </row>
+    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="1">
+        <f t="shared" ref="M3:BL8" ca="1" si="0">RANDBETWEEN(1,200)</f>
+        <v>3</v>
+      </c>
+      <c r="N3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="O3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="P3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="Q3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="R3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>119</v>
+      </c>
+      <c r="S3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="T3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="U3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>156</v>
+      </c>
+      <c r="V3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="W3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="X3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="Y3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>161</v>
+      </c>
+      <c r="Z3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>191</v>
+      </c>
+      <c r="AA3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="AB3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="AC3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>174</v>
+      </c>
+      <c r="AD3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="AE3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="AF3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="AG3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="AH3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="AI3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="AJ3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="AK3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="AL3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="AM3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>87</v>
+      </c>
+      <c r="AN3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>170</v>
+      </c>
+      <c r="AO3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="AP3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>98</v>
+      </c>
+      <c r="AQ3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="AR3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>113</v>
+      </c>
+      <c r="AS3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="AT3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="AU3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>127</v>
+      </c>
+      <c r="AV3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="AW3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="AX3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="AY3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>107</v>
+      </c>
+      <c r="AZ3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="BA3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>141</v>
+      </c>
+      <c r="BB3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="BC3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="BD3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>159</v>
+      </c>
+      <c r="BE3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="BF3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="BG3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>186</v>
+      </c>
+      <c r="BH3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>190</v>
+      </c>
+      <c r="BI3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="BJ3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>94</v>
+      </c>
+      <c r="BK3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>192</v>
+      </c>
+      <c r="BL3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1">
+        <v>7</v>
+      </c>
+      <c r="H4" s="1">
+        <v>8</v>
+      </c>
+      <c r="I4" s="1">
+        <v>9</v>
+      </c>
+      <c r="K4" s="18"/>
+      <c r="L4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="1">
+        <f t="shared" ref="M4:U11" ca="1" si="1">RANDBETWEEN(1,200)</f>
+        <v>154</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>103</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>145</v>
+      </c>
+      <c r="P4" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>101</v>
+      </c>
+      <c r="Q4" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="R4" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>117</v>
+      </c>
+      <c r="S4" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="T4" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="U4" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="V4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="W4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="X4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>114</v>
+      </c>
+      <c r="Y4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>177</v>
+      </c>
+      <c r="Z4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="AA4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="AB4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="AC4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="AD4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="AE4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>94</v>
+      </c>
+      <c r="AF4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="AG4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>118</v>
+      </c>
+      <c r="AH4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="AI4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="AJ4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>119</v>
+      </c>
+      <c r="AK4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>115</v>
+      </c>
+      <c r="AL4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>171</v>
+      </c>
+      <c r="AM4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>136</v>
+      </c>
+      <c r="AN4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>158</v>
+      </c>
+      <c r="AO4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>139</v>
+      </c>
+      <c r="AP4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>153</v>
+      </c>
+      <c r="AQ4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="AR4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="AS4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="AT4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="AU4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="AV4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="AW4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>106</v>
+      </c>
+      <c r="AX4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="AY4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>171</v>
+      </c>
+      <c r="AZ4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="BA4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="BB4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="BC4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>196</v>
+      </c>
+      <c r="BD4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>194</v>
+      </c>
+      <c r="BE4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>129</v>
+      </c>
+      <c r="BF4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>128</v>
+      </c>
+      <c r="BG4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="BH4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="BI4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="BJ4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>89</v>
+      </c>
+      <c r="BK4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>142</v>
+      </c>
+      <c r="BL4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <f ca="1">RANDBETWEEN(1,200)</f>
+        <v>11</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" ref="B5:I5" ca="1" si="2">RANDBETWEEN(1,200)</f>
+        <v>180</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>84</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>93</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>81</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>93</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>119</v>
+      </c>
+      <c r="K5" s="18"/>
+      <c r="L5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>141</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>159</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="Q5" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="R5" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>137</v>
+      </c>
+      <c r="S5" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="T5" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="U5" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>165</v>
+      </c>
+      <c r="V5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="W5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="X5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="Y5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="Z5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="AA5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>104</v>
+      </c>
+      <c r="AB5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>171</v>
+      </c>
+      <c r="AC5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="AD5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="AE5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>142</v>
+      </c>
+      <c r="AF5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="AG5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>173</v>
+      </c>
+      <c r="AH5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>184</v>
+      </c>
+      <c r="AI5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>129</v>
+      </c>
+      <c r="AJ5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="AK5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="AL5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>109</v>
+      </c>
+      <c r="AM5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>111</v>
+      </c>
+      <c r="AN5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="AO5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>107</v>
+      </c>
+      <c r="AP5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>149</v>
+      </c>
+      <c r="AQ5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>172</v>
+      </c>
+      <c r="AR5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="AS5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>198</v>
+      </c>
+      <c r="AT5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="AU5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="AV5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>194</v>
+      </c>
+      <c r="AW5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>173</v>
+      </c>
+      <c r="AX5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="AY5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="AZ5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="BA5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>116</v>
+      </c>
+      <c r="BB5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>154</v>
+      </c>
+      <c r="BC5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="BD5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="BE5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="BF5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>123</v>
+      </c>
+      <c r="BG5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>164</v>
+      </c>
+      <c r="BH5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>114</v>
+      </c>
+      <c r="BI5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="BJ5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="BK5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="BL5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="K6" s="18"/>
+      <c r="L6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>137</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>187</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>136</v>
+      </c>
+      <c r="P6" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="R6" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>164</v>
+      </c>
+      <c r="S6" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="T6" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="U6" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="V6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>173</v>
+      </c>
+      <c r="W6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="X6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="Y6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>195</v>
+      </c>
+      <c r="Z6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>188</v>
+      </c>
+      <c r="AA6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>131</v>
+      </c>
+      <c r="AB6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="AC6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>169</v>
+      </c>
+      <c r="AD6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="AE6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="AF6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="AG6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>170</v>
+      </c>
+      <c r="AH6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>189</v>
+      </c>
+      <c r="AI6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="AJ6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="AK6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>132</v>
+      </c>
+      <c r="AL6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="AM6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>142</v>
+      </c>
+      <c r="AN6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>132</v>
+      </c>
+      <c r="AO6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>149</v>
+      </c>
+      <c r="AP6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>189</v>
+      </c>
+      <c r="AQ6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="AR6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="AS6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="AT6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="AU6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>143</v>
+      </c>
+      <c r="AV6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="AW6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>126</v>
+      </c>
+      <c r="AX6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="AY6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>117</v>
+      </c>
+      <c r="AZ6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="BA6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>173</v>
+      </c>
+      <c r="BB6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="BC6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="BD6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="BE6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="BF6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="BG6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="BH6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="BI6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>139</v>
+      </c>
+      <c r="BJ6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="BK6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>191</v>
+      </c>
+      <c r="BL6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="K7" s="18"/>
+      <c r="L7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>192</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="O7" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>145</v>
+      </c>
+      <c r="P7" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="Q7" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="R7" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>114</v>
+      </c>
+      <c r="S7" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>195</v>
+      </c>
+      <c r="T7" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="U7" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="V7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>145</v>
+      </c>
+      <c r="W7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>148</v>
+      </c>
+      <c r="X7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>159</v>
+      </c>
+      <c r="Y7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>129</v>
+      </c>
+      <c r="Z7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="AA7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="AB7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="AC7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="AD7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>171</v>
+      </c>
+      <c r="AE7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="AF7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>119</v>
+      </c>
+      <c r="AG7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>193</v>
+      </c>
+      <c r="AH7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>196</v>
+      </c>
+      <c r="AI7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>159</v>
+      </c>
+      <c r="AJ7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="AK7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>156</v>
+      </c>
+      <c r="AL7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AM7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>106</v>
+      </c>
+      <c r="AN7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="AO7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>129</v>
+      </c>
+      <c r="AP7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>129</v>
+      </c>
+      <c r="AQ7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="AR7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>175</v>
+      </c>
+      <c r="AS7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>193</v>
+      </c>
+      <c r="AT7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>97</v>
+      </c>
+      <c r="AU7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="AV7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="AW7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="AX7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>127</v>
+      </c>
+      <c r="AY7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>137</v>
+      </c>
+      <c r="AZ7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="BA7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>148</v>
+      </c>
+      <c r="BB7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>97</v>
+      </c>
+      <c r="BC7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="BD7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="BE7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>147</v>
+      </c>
+      <c r="BF7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>195</v>
+      </c>
+      <c r="BG7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="BH7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="BI7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="BJ7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>143</v>
+      </c>
+      <c r="BK7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>178</v>
+      </c>
+      <c r="BL7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="K8" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="O8" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="P8" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>155</v>
+      </c>
+      <c r="Q8" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="R8" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>175</v>
+      </c>
+      <c r="S8" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="T8" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="U8" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>167</v>
+      </c>
+      <c r="V8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="W8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>159</v>
+      </c>
+      <c r="X8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="Y8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>174</v>
+      </c>
+      <c r="Z8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>156</v>
+      </c>
+      <c r="AA8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="AB8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="AC8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>141</v>
+      </c>
+      <c r="AD8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>193</v>
+      </c>
+      <c r="AE8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="AF8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="AG8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="AH8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="AI8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="AJ8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>134</v>
+      </c>
+      <c r="AK8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>108</v>
+      </c>
+      <c r="AL8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="AM8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="AN8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AO8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="AP8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>178</v>
+      </c>
+      <c r="AQ8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>171</v>
+      </c>
+      <c r="AR8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>189</v>
+      </c>
+      <c r="AS8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>155</v>
+      </c>
+      <c r="AT8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="AU8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>176</v>
+      </c>
+      <c r="AV8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>165</v>
+      </c>
+      <c r="AW8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="AX8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="AY8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="AZ8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>177</v>
+      </c>
+      <c r="BA8" s="1">
+        <f t="shared" ref="BA8:BL11" ca="1" si="3">RANDBETWEEN(1,200)</f>
+        <v>91</v>
+      </c>
+      <c r="BB8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>178</v>
+      </c>
+      <c r="BC8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="BD8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="BE8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>122</v>
+      </c>
+      <c r="BF8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="BG8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>68</v>
+      </c>
+      <c r="BH8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>144</v>
+      </c>
+      <c r="BI8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>174</v>
+      </c>
+      <c r="BJ8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>149</v>
+      </c>
+      <c r="BK8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>116</v>
+      </c>
+      <c r="BL8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="K9" s="19"/>
+      <c r="L9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>194</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>162</v>
+      </c>
+      <c r="O9" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="P9" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="Q9" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="R9" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>153</v>
+      </c>
+      <c r="S9" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="T9" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>153</v>
+      </c>
+      <c r="U9" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="V9" s="1">
+        <f t="shared" ref="V9:AK11" ca="1" si="4">RANDBETWEEN(1,200)</f>
+        <v>149</v>
+      </c>
+      <c r="W9" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="X9" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="Y9" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>186</v>
+      </c>
+      <c r="Z9" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>47</v>
+      </c>
+      <c r="AA9" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>178</v>
+      </c>
+      <c r="AB9" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>69</v>
+      </c>
+      <c r="AC9" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>46</v>
+      </c>
+      <c r="AD9" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>185</v>
+      </c>
+      <c r="AE9" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>143</v>
+      </c>
+      <c r="AF9" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>83</v>
+      </c>
+      <c r="AG9" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>196</v>
+      </c>
+      <c r="AH9" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>119</v>
+      </c>
+      <c r="AI9" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>182</v>
+      </c>
+      <c r="AJ9" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>87</v>
+      </c>
+      <c r="AK9" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>158</v>
+      </c>
+      <c r="AL9" s="1">
+        <f t="shared" ref="AL9:BA11" ca="1" si="5">RANDBETWEEN(1,200)</f>
+        <v>102</v>
+      </c>
+      <c r="AM9" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>135</v>
+      </c>
+      <c r="AN9" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>38</v>
+      </c>
+      <c r="AO9" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>192</v>
+      </c>
+      <c r="AP9" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>88</v>
+      </c>
+      <c r="AQ9" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>52</v>
+      </c>
+      <c r="AR9" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>42</v>
+      </c>
+      <c r="AS9" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>63</v>
+      </c>
+      <c r="AT9" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>65</v>
+      </c>
+      <c r="AU9" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>197</v>
+      </c>
+      <c r="AV9" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="AW9" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>147</v>
+      </c>
+      <c r="AX9" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>94</v>
+      </c>
+      <c r="AY9" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>195</v>
+      </c>
+      <c r="AZ9" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>106</v>
+      </c>
+      <c r="BA9" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>142</v>
+      </c>
+      <c r="BB9" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>182</v>
+      </c>
+      <c r="BC9" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>191</v>
+      </c>
+      <c r="BD9" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>177</v>
+      </c>
+      <c r="BE9" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>116</v>
+      </c>
+      <c r="BF9" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>110</v>
+      </c>
+      <c r="BG9" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>137</v>
+      </c>
+      <c r="BH9" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>79</v>
+      </c>
+      <c r="BI9" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>131</v>
+      </c>
+      <c r="BJ9" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="BK9" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>109</v>
+      </c>
+      <c r="BL9" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="K10" s="19"/>
+      <c r="L10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="O10" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="P10" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>176</v>
+      </c>
+      <c r="Q10" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="R10" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="S10" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="T10" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>114</v>
+      </c>
+      <c r="U10" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="V10" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>139</v>
+      </c>
+      <c r="W10" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>111</v>
+      </c>
+      <c r="X10" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>99</v>
+      </c>
+      <c r="Y10" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="Z10" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>104</v>
+      </c>
+      <c r="AA10" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>146</v>
+      </c>
+      <c r="AB10" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>137</v>
+      </c>
+      <c r="AC10" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>108</v>
+      </c>
+      <c r="AD10" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="AE10" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>124</v>
+      </c>
+      <c r="AF10" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>85</v>
+      </c>
+      <c r="AG10" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>49</v>
+      </c>
+      <c r="AH10" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>108</v>
+      </c>
+      <c r="AI10" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>165</v>
+      </c>
+      <c r="AJ10" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>148</v>
+      </c>
+      <c r="AK10" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>190</v>
+      </c>
+      <c r="AL10" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>54</v>
+      </c>
+      <c r="AM10" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="AN10" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>141</v>
+      </c>
+      <c r="AO10" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="AP10" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="AQ10" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>108</v>
+      </c>
+      <c r="AR10" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>76</v>
+      </c>
+      <c r="AS10" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="AT10" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="AU10" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="AV10" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>69</v>
+      </c>
+      <c r="AW10" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>174</v>
+      </c>
+      <c r="AX10" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="AY10" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>178</v>
+      </c>
+      <c r="AZ10" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>123</v>
+      </c>
+      <c r="BA10" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>35</v>
+      </c>
+      <c r="BB10" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>129</v>
+      </c>
+      <c r="BC10" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="BD10" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>140</v>
+      </c>
+      <c r="BE10" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>136</v>
+      </c>
+      <c r="BF10" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>164</v>
+      </c>
+      <c r="BG10" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="BH10" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>108</v>
+      </c>
+      <c r="BI10" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>170</v>
+      </c>
+      <c r="BJ10" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>117</v>
+      </c>
+      <c r="BK10" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>194</v>
+      </c>
+      <c r="BL10" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="K11" s="19"/>
+      <c r="L11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>172</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>171</v>
+      </c>
+      <c r="P11" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="Q11" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="R11" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="S11" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="T11" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="U11" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="V11" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>199</v>
+      </c>
+      <c r="W11" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>150</v>
+      </c>
+      <c r="X11" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>161</v>
+      </c>
+      <c r="Y11" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="Z11" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>189</v>
+      </c>
+      <c r="AA11" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>136</v>
+      </c>
+      <c r="AB11" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>197</v>
+      </c>
+      <c r="AC11" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>49</v>
+      </c>
+      <c r="AD11" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>180</v>
+      </c>
+      <c r="AE11" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="AF11" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>97</v>
+      </c>
+      <c r="AG11" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>186</v>
+      </c>
+      <c r="AH11" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="AI11" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>171</v>
+      </c>
+      <c r="AJ11" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>88</v>
+      </c>
+      <c r="AK11" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>161</v>
+      </c>
+      <c r="AL11" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>189</v>
+      </c>
+      <c r="AM11" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AN11" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>34</v>
+      </c>
+      <c r="AO11" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="AP11" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>117</v>
+      </c>
+      <c r="AQ11" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>91</v>
+      </c>
+      <c r="AR11" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>77</v>
+      </c>
+      <c r="AS11" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>49</v>
+      </c>
+      <c r="AT11" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>168</v>
+      </c>
+      <c r="AU11" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>48</v>
+      </c>
+      <c r="AV11" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>166</v>
+      </c>
+      <c r="AW11" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>94</v>
+      </c>
+      <c r="AX11" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>146</v>
+      </c>
+      <c r="AY11" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>65</v>
+      </c>
+      <c r="AZ11" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>59</v>
+      </c>
+      <c r="BA11" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>80</v>
+      </c>
+      <c r="BB11" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>89</v>
+      </c>
+      <c r="BC11" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>129</v>
+      </c>
+      <c r="BD11" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>95</v>
+      </c>
+      <c r="BE11" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>110</v>
+      </c>
+      <c r="BF11" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="BG11" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="BH11" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>195</v>
+      </c>
+      <c r="BI11" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>59</v>
+      </c>
+      <c r="BJ11" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>177</v>
+      </c>
+      <c r="BK11" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>197</v>
+      </c>
+      <c r="BL11" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="K8:K11"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="F2:I2"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>